<commit_message>
Backup BD y reinicio
</commit_message>
<xml_diff>
--- a/importados/cmd_import.xlsx
+++ b/importados/cmd_import.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B7092203-EC8F-4D64-894A-AC7CE69FC3C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6DCDEF3E-332C-46F4-B976-8FFBCF78236B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7380" yWindow="4470" windowWidth="28800" windowHeight="15345" xr2:uid="{4AEA10FA-AC70-4193-BE89-B72D9D8CA711}"/>
+    <workbookView xWindow="16620" yWindow="4470" windowWidth="28800" windowHeight="15345" xr2:uid="{4AEA10FA-AC70-4193-BE89-B72D9D8CA711}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,21 +25,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
-  <si>
-    <t>ID SENSOR</t>
-  </si>
-  <si>
-    <t>VALOR</t>
-  </si>
-  <si>
-    <t>TIMESTAMP</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>2024-05-13 13:45:00</t>
+    <t>0002</t>
+  </si>
+  <si>
+    <t>2025-08-18 00:01:00</t>
+  </si>
+  <si>
+    <t>ID_scada</t>
+  </si>
+  <si>
+    <t>valor</t>
+  </si>
+  <si>
+    <t>timestamp</t>
   </si>
 </sst>
 </file>
@@ -395,7 +398,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -407,29 +410,29 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="C1" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>200</v>
+      <c r="A2" s="1" t="s">
+        <v>1</v>
       </c>
       <c r="B2">
         <v>45</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>